<commit_message>
Bug fix in natural gas subsidy calculation
</commit_message>
<xml_diff>
--- a/InputData/fuels/BS/BAU Subsidies.xlsx
+++ b/InputData/fuels/BS/BAU Subsidies.xlsx
@@ -24059,8 +24059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ100"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AJ51" sqref="AJ51"/>
+    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H47" sqref="H47:AH47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -27891,128 +27891,128 @@
         <v>3.5031666E+16</v>
       </c>
       <c r="D47" s="7">
-        <f>'AEO Table 1'!E18*10^15</f>
+        <f>INDEX('AEO Table 1'!18:18,MATCH(Calculations!D34,'AEO Table 1'!13:13,0))*10^15</f>
+        <v>3.6033657E+16</v>
+      </c>
+      <c r="E47" s="7">
+        <f>INDEX('AEO Table 1'!18:18,MATCH(Calculations!E34,'AEO Table 1'!13:13,0))*10^15</f>
         <v>3.7331188E+16</v>
       </c>
-      <c r="E47" s="7">
-        <f>'AEO Table 1'!F18*10^15</f>
+      <c r="F47" s="7">
+        <f>INDEX('AEO Table 1'!18:18,MATCH(Calculations!F34,'AEO Table 1'!13:13,0))*10^15</f>
         <v>3.7590195E+16</v>
       </c>
-      <c r="F47" s="7">
-        <f>'AEO Table 1'!G18*10^15</f>
+      <c r="G47" s="7">
+        <f>INDEX('AEO Table 1'!18:18,MATCH(Calculations!G34,'AEO Table 1'!13:13,0))*10^15</f>
         <v>3.7847775E+16</v>
       </c>
-      <c r="G47" s="7">
-        <f>'AEO Table 1'!H18*10^15</f>
+      <c r="H47" s="7">
+        <f>INDEX('AEO Table 1'!18:18,MATCH(Calculations!H34,'AEO Table 1'!13:13,0))*10^15</f>
         <v>3.8332695E+16</v>
       </c>
-      <c r="H47" s="7">
-        <f>'AEO Table 1'!I18*10^15</f>
+      <c r="I47" s="7">
+        <f>INDEX('AEO Table 1'!18:18,MATCH(Calculations!I34,'AEO Table 1'!13:13,0))*10^15</f>
         <v>3.9291294E+16</v>
       </c>
-      <c r="I47" s="7">
-        <f>'AEO Table 1'!J18*10^15</f>
+      <c r="J47" s="7">
+        <f>INDEX('AEO Table 1'!18:18,MATCH(Calculations!J34,'AEO Table 1'!13:13,0))*10^15</f>
         <v>3.9964729E+16</v>
       </c>
-      <c r="J47" s="7">
-        <f>'AEO Table 1'!K18*10^15</f>
+      <c r="K47" s="7">
+        <f>INDEX('AEO Table 1'!18:18,MATCH(Calculations!K34,'AEO Table 1'!13:13,0))*10^15</f>
         <v>4.0147495E+16</v>
       </c>
-      <c r="K47" s="7">
-        <f>'AEO Table 1'!L18*10^15</f>
+      <c r="L47" s="7">
+        <f>INDEX('AEO Table 1'!18:18,MATCH(Calculations!L34,'AEO Table 1'!13:13,0))*10^15</f>
         <v>4.0689774E+16</v>
       </c>
-      <c r="L47" s="7">
-        <f>'AEO Table 1'!M18*10^15</f>
+      <c r="M47" s="7">
+        <f>INDEX('AEO Table 1'!18:18,MATCH(Calculations!M34,'AEO Table 1'!13:13,0))*10^15</f>
         <v>4.0984024E+16</v>
       </c>
-      <c r="M47" s="7">
-        <f>'AEO Table 1'!N18*10^15</f>
+      <c r="N47" s="7">
+        <f>INDEX('AEO Table 1'!18:18,MATCH(Calculations!N34,'AEO Table 1'!13:13,0))*10^15</f>
         <v>4.0933514E+16</v>
       </c>
-      <c r="N47" s="7">
-        <f>'AEO Table 1'!O18*10^15</f>
+      <c r="O47" s="7">
+        <f>INDEX('AEO Table 1'!18:18,MATCH(Calculations!O34,'AEO Table 1'!13:13,0))*10^15</f>
         <v>4.1105022E+16</v>
       </c>
-      <c r="O47" s="7">
-        <f>'AEO Table 1'!P18*10^15</f>
+      <c r="P47" s="7">
+        <f>INDEX('AEO Table 1'!18:18,MATCH(Calculations!P34,'AEO Table 1'!13:13,0))*10^15</f>
         <v>4.1415512E+16</v>
       </c>
-      <c r="P47" s="7">
-        <f>'AEO Table 1'!Q18*10^15</f>
+      <c r="Q47" s="7">
+        <f>INDEX('AEO Table 1'!18:18,MATCH(Calculations!Q34,'AEO Table 1'!13:13,0))*10^15</f>
         <v>4.1783867E+16</v>
       </c>
-      <c r="Q47" s="7">
-        <f>'AEO Table 1'!R18*10^15</f>
+      <c r="R47" s="7">
+        <f>INDEX('AEO Table 1'!18:18,MATCH(Calculations!R34,'AEO Table 1'!13:13,0))*10^15</f>
         <v>4.2303432E+16</v>
       </c>
-      <c r="R47" s="7">
-        <f>'AEO Table 1'!S18*10^15</f>
+      <c r="S47" s="7">
+        <f>INDEX('AEO Table 1'!18:18,MATCH(Calculations!S34,'AEO Table 1'!13:13,0))*10^15</f>
         <v>4.2534462E+16</v>
       </c>
-      <c r="S47" s="7">
-        <f>'AEO Table 1'!T18*10^15</f>
+      <c r="T47" s="7">
+        <f>INDEX('AEO Table 1'!18:18,MATCH(Calculations!T34,'AEO Table 1'!13:13,0))*10^15</f>
         <v>4.2787468E+16</v>
       </c>
-      <c r="T47" s="7">
-        <f>'AEO Table 1'!U18*10^15</f>
+      <c r="U47" s="7">
+        <f>INDEX('AEO Table 1'!18:18,MATCH(Calculations!U34,'AEO Table 1'!13:13,0))*10^15</f>
         <v>4.3062252E+16</v>
       </c>
-      <c r="U47" s="7">
-        <f>'AEO Table 1'!V18*10^15</f>
+      <c r="V47" s="7">
+        <f>INDEX('AEO Table 1'!18:18,MATCH(Calculations!V34,'AEO Table 1'!13:13,0))*10^15</f>
         <v>4.3329517E+16</v>
       </c>
-      <c r="V47" s="7">
-        <f>'AEO Table 1'!W18*10^15</f>
+      <c r="W47" s="7">
+        <f>INDEX('AEO Table 1'!18:18,MATCH(Calculations!W34,'AEO Table 1'!13:13,0))*10^15</f>
         <v>4.3569817E+16</v>
       </c>
-      <c r="W47" s="7">
-        <f>'AEO Table 1'!X18*10^15</f>
+      <c r="X47" s="7">
+        <f>INDEX('AEO Table 1'!18:18,MATCH(Calculations!X34,'AEO Table 1'!13:13,0))*10^15</f>
         <v>4.3935242E+16</v>
       </c>
-      <c r="X47" s="7">
-        <f>'AEO Table 1'!Y18*10^15</f>
+      <c r="Y47" s="7">
+        <f>INDEX('AEO Table 1'!18:18,MATCH(Calculations!Y34,'AEO Table 1'!13:13,0))*10^15</f>
         <v>4.4149738E+16</v>
       </c>
-      <c r="Y47" s="7">
-        <f>'AEO Table 1'!Z18*10^15</f>
+      <c r="Z47" s="7">
+        <f>INDEX('AEO Table 1'!18:18,MATCH(Calculations!Z34,'AEO Table 1'!13:13,0))*10^15</f>
         <v>4.4370525E+16</v>
       </c>
-      <c r="Z47" s="7">
-        <f>'AEO Table 1'!AA18*10^15</f>
+      <c r="AA47" s="7">
+        <f>INDEX('AEO Table 1'!18:18,MATCH(Calculations!AA34,'AEO Table 1'!13:13,0))*10^15</f>
         <v>4.4607227E+16</v>
       </c>
-      <c r="AA47" s="7">
-        <f>'AEO Table 1'!AB18*10^15</f>
+      <c r="AB47" s="7">
+        <f>INDEX('AEO Table 1'!18:18,MATCH(Calculations!AB34,'AEO Table 1'!13:13,0))*10^15</f>
         <v>4.4817394E+16</v>
       </c>
-      <c r="AB47" s="7">
-        <f>'AEO Table 1'!AC18*10^15</f>
+      <c r="AC47" s="7">
+        <f>INDEX('AEO Table 1'!18:18,MATCH(Calculations!AC34,'AEO Table 1'!13:13,0))*10^15</f>
         <v>4.4978981E+16</v>
       </c>
-      <c r="AC47" s="7">
-        <f>'AEO Table 1'!AD18*10^15</f>
+      <c r="AD47" s="7">
+        <f>INDEX('AEO Table 1'!18:18,MATCH(Calculations!AD34,'AEO Table 1'!13:13,0))*10^15</f>
         <v>4.5196522E+16</v>
       </c>
-      <c r="AD47" s="7">
-        <f>'AEO Table 1'!AE18*10^15</f>
+      <c r="AE47" s="7">
+        <f>INDEX('AEO Table 1'!18:18,MATCH(Calculations!AE34,'AEO Table 1'!13:13,0))*10^15</f>
         <v>4.5565365E+16</v>
       </c>
-      <c r="AE47" s="7">
-        <f>'AEO Table 1'!AF18*10^15</f>
+      <c r="AF47" s="7">
+        <f>INDEX('AEO Table 1'!18:18,MATCH(Calculations!AF34,'AEO Table 1'!13:13,0))*10^15</f>
         <v>4.6018311E+16</v>
       </c>
-      <c r="AF47" s="7">
-        <f>'AEO Table 1'!AG18*10^15</f>
+      <c r="AG47" s="7">
+        <f>INDEX('AEO Table 1'!18:18,MATCH(Calculations!AG34,'AEO Table 1'!13:13,0))*10^15</f>
         <v>4.6380791E+16</v>
       </c>
-      <c r="AG47" s="7">
-        <f>'AEO Table 1'!AH18*10^15</f>
+      <c r="AH47" s="7">
+        <f>INDEX('AEO Table 1'!18:18,MATCH(Calculations!AH34,'AEO Table 1'!13:13,0))*10^15</f>
         <v>4.6616814E+16</v>
-      </c>
-      <c r="AH47" s="7">
-        <f>'AEO Table 1'!AI18*10^15</f>
-        <v>9259000000000</v>
       </c>
       <c r="AI47" s="7"/>
       <c r="AJ47" s="7"/>
@@ -28165,127 +28165,127 @@
       </c>
       <c r="D49" s="7">
         <f>D46*(D47/SUM(D47:D48))/D47</f>
-        <v>2.2489652573322277E-8</v>
+        <v>2.2902189160885848E-8</v>
       </c>
       <c r="E49" s="7">
         <f t="shared" ref="E49:P49" si="84">E46*(E47/SUM(E47:E48))/E47</f>
-        <v>2.2049985520509512E-8</v>
+        <v>2.2127994906299485E-8</v>
       </c>
       <c r="F49" s="7">
         <f t="shared" si="84"/>
-        <v>2.1517569633545032E-8</v>
+        <v>2.1591440289411669E-8</v>
       </c>
       <c r="G49" s="7">
         <f t="shared" si="84"/>
-        <v>2.1325093387454493E-8</v>
+        <v>2.1462092605432069E-8</v>
       </c>
       <c r="H49" s="7">
         <f t="shared" si="84"/>
-        <v>2.0982281357083705E-8</v>
+        <v>2.1246068264246853E-8</v>
       </c>
       <c r="I49" s="7">
         <f t="shared" si="84"/>
-        <v>2.0773777829601092E-8</v>
+        <v>2.0954736062681669E-8</v>
       </c>
       <c r="J49" s="7">
         <f t="shared" si="84"/>
-        <v>2.0642450396478403E-8</v>
+        <v>2.0690635797566348E-8</v>
       </c>
       <c r="K49" s="7">
         <f t="shared" si="84"/>
-        <v>2.0466969059817563E-8</v>
+        <v>2.0608157935223373E-8</v>
       </c>
       <c r="L49" s="7">
         <f t="shared" si="84"/>
-        <v>2.0438746974103441E-8</v>
+        <v>2.051490668205842E-8</v>
       </c>
       <c r="M49" s="7">
         <f t="shared" si="84"/>
-        <v>2.0444342643396718E-8</v>
+        <v>2.0431319017578943E-8</v>
       </c>
       <c r="N49" s="7">
         <f t="shared" si="84"/>
-        <v>2.0352812486686656E-8</v>
+        <v>2.0396762097115002E-8</v>
       </c>
       <c r="O49" s="7">
         <f t="shared" si="84"/>
-        <v>2.0240953811717699E-8</v>
+        <v>2.0319782196017565E-8</v>
       </c>
       <c r="P49" s="7">
         <f t="shared" si="84"/>
-        <v>2.0108316550233104E-8</v>
+        <v>2.0200678528322213E-8</v>
       </c>
       <c r="Q49" s="7">
         <f t="shared" ref="Q49:AH49" si="85">Q46*(Q47/SUM(Q47:Q48))/Q47</f>
-        <v>1.999148412138119E-8</v>
+        <v>2.0120489689497254E-8</v>
       </c>
       <c r="R49" s="7">
         <f t="shared" si="85"/>
-        <v>1.9978536146018535E-8</v>
+        <v>2.0035620860356275E-8</v>
       </c>
       <c r="S49" s="7">
         <f t="shared" si="85"/>
-        <v>1.9951565972550047E-8</v>
+        <v>2.0013928706037249E-8</v>
       </c>
       <c r="T49" s="7">
         <f t="shared" si="85"/>
-        <v>1.9956559497519459E-8</v>
+        <v>2.0024342431187308E-8</v>
       </c>
       <c r="U49" s="7">
         <f t="shared" si="85"/>
-        <v>2.0006639734436314E-8</v>
+        <v>2.0072893597940164E-8</v>
       </c>
       <c r="V49" s="7">
         <f t="shared" si="85"/>
-        <v>2.003719373164842E-8</v>
+        <v>2.0096925486741025E-8</v>
       </c>
       <c r="W49" s="7">
         <f t="shared" si="85"/>
-        <v>1.998971615479153E-8</v>
+        <v>2.008026005572942E-8</v>
       </c>
       <c r="X49" s="7">
         <f t="shared" si="85"/>
-        <v>1.9853185448507236E-8</v>
+        <v>1.9905510263010773E-8</v>
       </c>
       <c r="Y49" s="7">
         <f t="shared" si="85"/>
-        <v>1.9750394032552553E-8</v>
+        <v>1.9803700585503743E-8</v>
       </c>
       <c r="Z49" s="7">
         <f t="shared" si="85"/>
-        <v>1.9689091022120882E-8</v>
+        <v>1.9745896397450186E-8</v>
       </c>
       <c r="AA49" s="7">
         <f t="shared" si="85"/>
-        <v>1.9661955160547147E-8</v>
+        <v>1.971223711222151E-8</v>
       </c>
       <c r="AB49" s="7">
         <f t="shared" si="85"/>
-        <v>1.9711175071846327E-8</v>
+        <v>1.9750005406868765E-8</v>
       </c>
       <c r="AC49" s="7">
         <f t="shared" si="85"/>
-        <v>1.9782091470412751E-8</v>
+        <v>1.9834781170328004E-8</v>
       </c>
       <c r="AD49" s="7">
         <f t="shared" si="85"/>
-        <v>1.9839775686107512E-8</v>
+        <v>1.9929801334573316E-8</v>
       </c>
       <c r="AE49" s="7">
         <f t="shared" si="85"/>
-        <v>1.9879367579888E-8</v>
+        <v>1.9990478609077307E-8</v>
       </c>
       <c r="AF49" s="7">
         <f t="shared" si="85"/>
-        <v>1.992033293221325E-8</v>
+        <v>2.0009520085000442E-8</v>
       </c>
       <c r="AG49" s="7">
         <f t="shared" si="85"/>
-        <v>2.0027454425734876E-8</v>
+        <v>2.0086062827791064E-8</v>
       </c>
       <c r="AH49" s="7">
         <f t="shared" si="85"/>
-        <v>4.9096305221182947E-8</v>
+        <v>2.035075455070509E-8</v>
       </c>
       <c r="AI49" s="7"/>
       <c r="AJ49" s="7"/>
@@ -28488,127 +28488,127 @@
       </c>
       <c r="D53" s="7">
         <f t="shared" ref="D53:AH53" si="105">D47</f>
-        <v>3.7331188E+16</v>
+        <v>3.6033657E+16</v>
       </c>
       <c r="E53" s="7">
         <f t="shared" si="105"/>
-        <v>3.7590195E+16</v>
+        <v>3.7331188E+16</v>
       </c>
       <c r="F53" s="7">
         <f t="shared" si="105"/>
-        <v>3.7847775E+16</v>
+        <v>3.7590195E+16</v>
       </c>
       <c r="G53" s="7">
         <f t="shared" si="105"/>
-        <v>3.8332695E+16</v>
+        <v>3.7847775E+16</v>
       </c>
       <c r="H53" s="7">
         <f t="shared" si="105"/>
-        <v>3.9291294E+16</v>
+        <v>3.8332695E+16</v>
       </c>
       <c r="I53" s="7">
         <f t="shared" si="105"/>
-        <v>3.9964729E+16</v>
+        <v>3.9291294E+16</v>
       </c>
       <c r="J53" s="7">
         <f t="shared" si="105"/>
-        <v>4.0147495E+16</v>
+        <v>3.9964729E+16</v>
       </c>
       <c r="K53" s="7">
         <f t="shared" si="105"/>
-        <v>4.0689774E+16</v>
+        <v>4.0147495E+16</v>
       </c>
       <c r="L53" s="7">
         <f t="shared" si="105"/>
-        <v>4.0984024E+16</v>
+        <v>4.0689774E+16</v>
       </c>
       <c r="M53" s="7">
         <f t="shared" si="105"/>
-        <v>4.0933514E+16</v>
+        <v>4.0984024E+16</v>
       </c>
       <c r="N53" s="7">
         <f t="shared" si="105"/>
-        <v>4.1105022E+16</v>
+        <v>4.0933514E+16</v>
       </c>
       <c r="O53" s="7">
         <f t="shared" si="105"/>
-        <v>4.1415512E+16</v>
+        <v>4.1105022E+16</v>
       </c>
       <c r="P53" s="7">
         <f t="shared" si="105"/>
-        <v>4.1783867E+16</v>
+        <v>4.1415512E+16</v>
       </c>
       <c r="Q53" s="7">
         <f t="shared" si="105"/>
-        <v>4.2303432E+16</v>
+        <v>4.1783867E+16</v>
       </c>
       <c r="R53" s="7">
         <f t="shared" si="105"/>
-        <v>4.2534462E+16</v>
+        <v>4.2303432E+16</v>
       </c>
       <c r="S53" s="7">
         <f t="shared" si="105"/>
-        <v>4.2787468E+16</v>
+        <v>4.2534462E+16</v>
       </c>
       <c r="T53" s="7">
         <f t="shared" si="105"/>
-        <v>4.3062252E+16</v>
+        <v>4.2787468E+16</v>
       </c>
       <c r="U53" s="7">
         <f t="shared" si="105"/>
-        <v>4.3329517E+16</v>
+        <v>4.3062252E+16</v>
       </c>
       <c r="V53" s="7">
         <f t="shared" si="105"/>
-        <v>4.3569817E+16</v>
+        <v>4.3329517E+16</v>
       </c>
       <c r="W53" s="7">
         <f t="shared" si="105"/>
-        <v>4.3935242E+16</v>
+        <v>4.3569817E+16</v>
       </c>
       <c r="X53" s="7">
         <f t="shared" si="105"/>
-        <v>4.4149738E+16</v>
+        <v>4.3935242E+16</v>
       </c>
       <c r="Y53" s="7">
         <f t="shared" si="105"/>
-        <v>4.4370525E+16</v>
+        <v>4.4149738E+16</v>
       </c>
       <c r="Z53" s="7">
         <f t="shared" si="105"/>
-        <v>4.4607227E+16</v>
+        <v>4.4370525E+16</v>
       </c>
       <c r="AA53" s="7">
         <f t="shared" si="105"/>
-        <v>4.4817394E+16</v>
+        <v>4.4607227E+16</v>
       </c>
       <c r="AB53" s="7">
         <f t="shared" si="105"/>
-        <v>4.4978981E+16</v>
+        <v>4.4817394E+16</v>
       </c>
       <c r="AC53" s="7">
         <f t="shared" si="105"/>
-        <v>4.5196522E+16</v>
+        <v>4.4978981E+16</v>
       </c>
       <c r="AD53" s="7">
         <f t="shared" si="105"/>
-        <v>4.5565365E+16</v>
+        <v>4.5196522E+16</v>
       </c>
       <c r="AE53" s="7">
         <f t="shared" si="105"/>
-        <v>4.6018311E+16</v>
+        <v>4.5565365E+16</v>
       </c>
       <c r="AF53" s="7">
         <f t="shared" si="105"/>
-        <v>4.6380791E+16</v>
+        <v>4.6018311E+16</v>
       </c>
       <c r="AG53" s="7">
         <f t="shared" si="105"/>
-        <v>4.6616814E+16</v>
+        <v>4.6380791E+16</v>
       </c>
       <c r="AH53" s="7">
         <f t="shared" si="105"/>
-        <v>9259000000000</v>
+        <v>4.6616814E+16</v>
       </c>
       <c r="AI53" s="7"/>
       <c r="AJ53" s="7"/>
@@ -28762,127 +28762,127 @@
       </c>
       <c r="D55" s="7">
         <f t="shared" si="107"/>
-        <v>1.9435502223858752E-9</v>
+        <v>1.9792015324222333E-9</v>
       </c>
       <c r="E55" s="7">
         <f t="shared" si="107"/>
-        <v>1.9055543042415622E-9</v>
+        <v>1.9122958560999554E-9</v>
       </c>
       <c r="F55" s="7">
         <f t="shared" si="107"/>
-        <v>1.8595430547508048E-9</v>
+        <v>1.8659269385911315E-9</v>
       </c>
       <c r="G55" s="7">
         <f t="shared" si="107"/>
-        <v>1.8429093050886598E-9</v>
+        <v>1.854748743679314E-9</v>
       </c>
       <c r="H55" s="7">
         <f t="shared" si="107"/>
-        <v>1.813283574068962E-9</v>
+        <v>1.8360799734534313E-9</v>
       </c>
       <c r="I55" s="7">
         <f t="shared" si="107"/>
-        <v>1.7952647507062668E-9</v>
+        <v>1.8109031165280453E-9</v>
       </c>
       <c r="J55" s="7">
         <f t="shared" si="107"/>
-        <v>1.7839154663623308E-9</v>
+        <v>1.7880796368267211E-9</v>
       </c>
       <c r="K55" s="7">
         <f t="shared" si="107"/>
-        <v>1.7687504125768261E-9</v>
+        <v>1.7809519203279457E-9</v>
       </c>
       <c r="L55" s="7">
         <f t="shared" si="107"/>
-        <v>1.7663114668978281E-9</v>
+        <v>1.7728931700544315E-9</v>
       </c>
       <c r="M55" s="7">
         <f t="shared" si="107"/>
-        <v>1.766795043256506E-9</v>
+        <v>1.7656695447290443E-9</v>
       </c>
       <c r="N55" s="7">
         <f t="shared" si="107"/>
-        <v>1.7588850297136612E-9</v>
+        <v>1.7626831441951235E-9</v>
       </c>
       <c r="O55" s="7">
         <f t="shared" si="107"/>
-        <v>1.74921823064227E-9</v>
+        <v>1.7560305601496659E-9</v>
       </c>
       <c r="P55" s="7">
         <f t="shared" si="107"/>
-        <v>1.7377557512547125E-9</v>
+        <v>1.7457376505957467E-9</v>
       </c>
       <c r="Q55" s="7">
         <f t="shared" si="107"/>
-        <v>1.7276591216008431E-9</v>
+        <v>1.7388077509442068E-9</v>
       </c>
       <c r="R55" s="7">
         <f t="shared" si="107"/>
-        <v>1.7265401607670338E-9</v>
+        <v>1.7314734076851101E-9</v>
       </c>
       <c r="S55" s="7">
         <f t="shared" si="107"/>
-        <v>1.724209405035189E-9</v>
+        <v>1.7295987770649471E-9</v>
       </c>
       <c r="T55" s="7">
         <f t="shared" si="107"/>
-        <v>1.7246409442300763E-9</v>
+        <v>1.730498728621125E-9</v>
       </c>
       <c r="U55" s="7">
         <f t="shared" si="107"/>
-        <v>1.7289688659389402E-9</v>
+        <v>1.7346945084639646E-9</v>
       </c>
       <c r="V55" s="7">
         <f t="shared" si="107"/>
-        <v>1.7316093348338138E-9</v>
+        <v>1.7367713383603353E-9</v>
       </c>
       <c r="W55" s="7">
         <f t="shared" si="107"/>
-        <v>1.7275063343646999E-9</v>
+        <v>1.7353311159272332E-9</v>
       </c>
       <c r="X55" s="7">
         <f t="shared" si="107"/>
-        <v>1.7157073844388968E-9</v>
+        <v>1.7202292819885853E-9</v>
       </c>
       <c r="Y55" s="7">
         <f t="shared" si="107"/>
-        <v>1.7068241756526897E-9</v>
+        <v>1.7114309147966197E-9</v>
       </c>
       <c r="Z55" s="7">
         <f t="shared" si="107"/>
-        <v>1.70152638462773E-9</v>
+        <v>1.70643549113767E-9</v>
       </c>
       <c r="AA55" s="7">
         <f t="shared" si="107"/>
-        <v>1.699181310170741E-9</v>
+        <v>1.7035266640191428E-9</v>
       </c>
       <c r="AB55" s="7">
         <f t="shared" si="107"/>
-        <v>1.7034348827521511E-9</v>
+        <v>1.7067905907170537E-9</v>
       </c>
       <c r="AC55" s="7">
         <f t="shared" si="107"/>
-        <v>1.70956346040604E-9</v>
+        <v>1.7141168912629136E-9</v>
       </c>
       <c r="AD55" s="7">
         <f t="shared" si="107"/>
-        <v>1.714548516083365E-9</v>
+        <v>1.7223285103952246E-9</v>
       </c>
       <c r="AE55" s="7">
         <f t="shared" si="107"/>
-        <v>1.7179700377680988E-9</v>
+        <v>1.7275722254758164E-9</v>
       </c>
       <c r="AF55" s="7">
         <f t="shared" si="107"/>
-        <v>1.7215102534011446E-9</v>
+        <v>1.7292177851234949E-9</v>
       </c>
       <c r="AG55" s="7">
         <f t="shared" si="107"/>
-        <v>1.7307676664215321E-9</v>
+        <v>1.7358325900560179E-9</v>
       </c>
       <c r="AH55" s="7">
         <f t="shared" si="107"/>
-        <v>4.2428905746701309E-9</v>
+        <v>1.7587071833942671E-9</v>
       </c>
       <c r="AI55" s="7"/>
       <c r="AJ55" s="7"/>
@@ -29064,127 +29064,127 @@
       </c>
       <c r="D59" s="7">
         <f t="shared" ref="D59:AH59" si="127">D47</f>
-        <v>3.7331188E+16</v>
+        <v>3.6033657E+16</v>
       </c>
       <c r="E59" s="7">
         <f t="shared" si="127"/>
-        <v>3.7590195E+16</v>
+        <v>3.7331188E+16</v>
       </c>
       <c r="F59" s="7">
         <f t="shared" si="127"/>
-        <v>3.7847775E+16</v>
+        <v>3.7590195E+16</v>
       </c>
       <c r="G59" s="7">
         <f t="shared" si="127"/>
-        <v>3.8332695E+16</v>
+        <v>3.7847775E+16</v>
       </c>
       <c r="H59" s="7">
         <f t="shared" si="127"/>
-        <v>3.9291294E+16</v>
+        <v>3.8332695E+16</v>
       </c>
       <c r="I59" s="7">
         <f t="shared" si="127"/>
-        <v>3.9964729E+16</v>
+        <v>3.9291294E+16</v>
       </c>
       <c r="J59" s="7">
         <f t="shared" si="127"/>
-        <v>4.0147495E+16</v>
+        <v>3.9964729E+16</v>
       </c>
       <c r="K59" s="7">
         <f t="shared" si="127"/>
-        <v>4.0689774E+16</v>
+        <v>4.0147495E+16</v>
       </c>
       <c r="L59" s="7">
         <f t="shared" si="127"/>
-        <v>4.0984024E+16</v>
+        <v>4.0689774E+16</v>
       </c>
       <c r="M59" s="7">
         <f t="shared" si="127"/>
-        <v>4.0933514E+16</v>
+        <v>4.0984024E+16</v>
       </c>
       <c r="N59" s="7">
         <f t="shared" si="127"/>
-        <v>4.1105022E+16</v>
+        <v>4.0933514E+16</v>
       </c>
       <c r="O59" s="7">
         <f t="shared" si="127"/>
-        <v>4.1415512E+16</v>
+        <v>4.1105022E+16</v>
       </c>
       <c r="P59" s="7">
         <f t="shared" si="127"/>
-        <v>4.1783867E+16</v>
+        <v>4.1415512E+16</v>
       </c>
       <c r="Q59" s="7">
         <f t="shared" si="127"/>
-        <v>4.2303432E+16</v>
+        <v>4.1783867E+16</v>
       </c>
       <c r="R59" s="7">
         <f t="shared" si="127"/>
-        <v>4.2534462E+16</v>
+        <v>4.2303432E+16</v>
       </c>
       <c r="S59" s="7">
         <f t="shared" si="127"/>
-        <v>4.2787468E+16</v>
+        <v>4.2534462E+16</v>
       </c>
       <c r="T59" s="7">
         <f t="shared" si="127"/>
-        <v>4.3062252E+16</v>
+        <v>4.2787468E+16</v>
       </c>
       <c r="U59" s="7">
         <f t="shared" si="127"/>
-        <v>4.3329517E+16</v>
+        <v>4.3062252E+16</v>
       </c>
       <c r="V59" s="7">
         <f t="shared" si="127"/>
-        <v>4.3569817E+16</v>
+        <v>4.3329517E+16</v>
       </c>
       <c r="W59" s="7">
         <f t="shared" si="127"/>
-        <v>4.3935242E+16</v>
+        <v>4.3569817E+16</v>
       </c>
       <c r="X59" s="7">
         <f t="shared" si="127"/>
-        <v>4.4149738E+16</v>
+        <v>4.3935242E+16</v>
       </c>
       <c r="Y59" s="7">
         <f t="shared" si="127"/>
-        <v>4.4370525E+16</v>
+        <v>4.4149738E+16</v>
       </c>
       <c r="Z59" s="7">
         <f t="shared" si="127"/>
-        <v>4.4607227E+16</v>
+        <v>4.4370525E+16</v>
       </c>
       <c r="AA59" s="7">
         <f t="shared" si="127"/>
-        <v>4.4817394E+16</v>
+        <v>4.4607227E+16</v>
       </c>
       <c r="AB59" s="7">
         <f t="shared" si="127"/>
-        <v>4.4978981E+16</v>
+        <v>4.4817394E+16</v>
       </c>
       <c r="AC59" s="7">
         <f t="shared" si="127"/>
-        <v>4.5196522E+16</v>
+        <v>4.4978981E+16</v>
       </c>
       <c r="AD59" s="7">
         <f t="shared" si="127"/>
-        <v>4.5565365E+16</v>
+        <v>4.5196522E+16</v>
       </c>
       <c r="AE59" s="7">
         <f t="shared" si="127"/>
-        <v>4.6018311E+16</v>
+        <v>4.5565365E+16</v>
       </c>
       <c r="AF59" s="7">
         <f t="shared" si="127"/>
-        <v>4.6380791E+16</v>
+        <v>4.6018311E+16</v>
       </c>
       <c r="AG59" s="7">
         <f t="shared" si="127"/>
-        <v>4.6616814E+16</v>
+        <v>4.6380791E+16</v>
       </c>
       <c r="AH59" s="7">
         <f t="shared" si="127"/>
-        <v>9259000000000</v>
+        <v>4.6616814E+16</v>
       </c>
       <c r="AI59" s="7"/>
       <c r="AJ59" s="7"/>
@@ -29338,127 +29338,127 @@
       </c>
       <c r="D61" s="7">
         <f t="shared" si="129"/>
-        <v>1.6659001906164646E-8</v>
+        <v>1.6964584563619144E-8</v>
       </c>
       <c r="E61" s="7">
         <f t="shared" si="129"/>
-        <v>1.633332260778482E-8</v>
+        <v>1.6391107337999616E-8</v>
       </c>
       <c r="F61" s="7">
         <f t="shared" si="129"/>
-        <v>1.5938940469292614E-8</v>
+        <v>1.599365947363827E-8</v>
       </c>
       <c r="G61" s="7">
         <f t="shared" si="129"/>
-        <v>1.5796365472188511E-8</v>
+        <v>1.5897846374394123E-8</v>
       </c>
       <c r="H61" s="7">
         <f t="shared" si="129"/>
-        <v>1.5542430634876816E-8</v>
+        <v>1.5737828343886555E-8</v>
       </c>
       <c r="I61" s="7">
         <f t="shared" si="129"/>
-        <v>1.5387983577482287E-8</v>
+        <v>1.552202671309753E-8</v>
       </c>
       <c r="J61" s="7">
         <f t="shared" si="129"/>
-        <v>1.5290703997391406E-8</v>
+        <v>1.5326396887086182E-8</v>
       </c>
       <c r="K61" s="7">
         <f t="shared" si="129"/>
-        <v>1.5160717822087081E-8</v>
+        <v>1.5265302174239533E-8</v>
       </c>
       <c r="L61" s="7">
         <f t="shared" si="129"/>
-        <v>1.5139812573409957E-8</v>
+        <v>1.5196227171895125E-8</v>
       </c>
       <c r="M61" s="7">
         <f t="shared" si="129"/>
-        <v>1.5143957513627196E-8</v>
+        <v>1.5134310383391806E-8</v>
       </c>
       <c r="N61" s="7">
         <f t="shared" si="129"/>
-        <v>1.5076157397545668E-8</v>
+        <v>1.5108712664529631E-8</v>
       </c>
       <c r="O61" s="7">
         <f t="shared" si="129"/>
-        <v>1.4993299119790887E-8</v>
+        <v>1.5051690515568565E-8</v>
       </c>
       <c r="P61" s="7">
         <f t="shared" si="129"/>
-        <v>1.4895049296468962E-8</v>
+        <v>1.4963465576534973E-8</v>
       </c>
       <c r="Q61" s="7">
         <f t="shared" si="129"/>
-        <v>1.4808506756578655E-8</v>
+        <v>1.4904066436664629E-8</v>
       </c>
       <c r="R61" s="7">
         <f t="shared" si="129"/>
-        <v>1.4798915663717432E-8</v>
+        <v>1.4841200637300945E-8</v>
       </c>
       <c r="S61" s="7">
         <f t="shared" si="129"/>
-        <v>1.4778937757444477E-8</v>
+        <v>1.4825132374842405E-8</v>
       </c>
       <c r="T61" s="7">
         <f t="shared" si="129"/>
-        <v>1.4782636664829227E-8</v>
+        <v>1.4832846245323927E-8</v>
       </c>
       <c r="U61" s="7">
         <f t="shared" si="129"/>
-        <v>1.4819733136619488E-8</v>
+        <v>1.4868810072548269E-8</v>
       </c>
       <c r="V61" s="7">
         <f t="shared" si="129"/>
-        <v>1.4842365727146975E-8</v>
+        <v>1.4886611471660016E-8</v>
       </c>
       <c r="W61" s="7">
         <f t="shared" si="129"/>
-        <v>1.4807197151697427E-8</v>
+        <v>1.4874266707947714E-8</v>
       </c>
       <c r="X61" s="7">
         <f t="shared" si="129"/>
-        <v>1.4706063295190545E-8</v>
+        <v>1.4744822417045016E-8</v>
       </c>
       <c r="Y61" s="7">
         <f t="shared" si="129"/>
-        <v>1.4629921505594481E-8</v>
+        <v>1.4669407841113884E-8</v>
       </c>
       <c r="Z61" s="7">
         <f t="shared" si="129"/>
-        <v>1.4584511868237685E-8</v>
+        <v>1.4626589924037171E-8</v>
       </c>
       <c r="AA61" s="7">
         <f t="shared" si="129"/>
-        <v>1.4564411230034924E-8</v>
+        <v>1.4601657120164081E-8</v>
       </c>
       <c r="AB61" s="7">
         <f t="shared" si="129"/>
-        <v>1.4600870423589869E-8</v>
+        <v>1.4629633634717602E-8</v>
       </c>
       <c r="AC61" s="7">
         <f t="shared" si="129"/>
-        <v>1.465340108919463E-8</v>
+        <v>1.4692430496539258E-8</v>
       </c>
       <c r="AD61" s="7">
         <f t="shared" si="129"/>
-        <v>1.4696130137857414E-8</v>
+        <v>1.4762815803387638E-8</v>
       </c>
       <c r="AE61" s="7">
         <f t="shared" si="129"/>
-        <v>1.4725457466583703E-8</v>
+        <v>1.4807761932649854E-8</v>
       </c>
       <c r="AF61" s="7">
         <f t="shared" si="129"/>
-        <v>1.4755802172009814E-8</v>
+        <v>1.4821866729629954E-8</v>
       </c>
       <c r="AG61" s="7">
         <f t="shared" si="129"/>
-        <v>1.4835151426470275E-8</v>
+        <v>1.4878565057623009E-8</v>
       </c>
       <c r="AH61" s="7">
         <f t="shared" si="129"/>
-        <v>3.636763349717255E-8</v>
+        <v>1.5074633000522288E-8</v>
       </c>
       <c r="AI61" s="7"/>
       <c r="AJ61" s="7"/>
@@ -33288,8 +33288,8 @@
   </sheetPr>
   <dimension ref="A1:AI22"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="AG5" sqref="AG5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -33645,127 +33645,127 @@
       </c>
       <c r="C4" s="28">
         <f>SUM(Calculations!D49,Calculations!D55,Calculations!D61)</f>
-        <v>4.1092204701872802E-8</v>
+        <v>4.1845975256927227E-8</v>
       </c>
       <c r="D4" s="28">
         <f>SUM(Calculations!E49,Calculations!E55,Calculations!E61)</f>
-        <v>4.0288862432535892E-8</v>
+        <v>4.0431398100399054E-8</v>
       </c>
       <c r="E4" s="28">
         <f>SUM(Calculations!F49,Calculations!F55,Calculations!F61)</f>
-        <v>3.9316053157588455E-8</v>
+        <v>3.9451026701641067E-8</v>
       </c>
       <c r="F4" s="28">
         <f>SUM(Calculations!G49,Calculations!G55,Calculations!G61)</f>
-        <v>3.8964368164731665E-8</v>
+        <v>3.9214687723505507E-8</v>
       </c>
       <c r="G4" s="28">
         <f>SUM(Calculations!H49,Calculations!H55,Calculations!H61)</f>
-        <v>3.833799556602948E-8</v>
+        <v>3.8819976581586842E-8</v>
       </c>
       <c r="H4" s="28">
         <f>SUM(Calculations!I49,Calculations!I55,Calculations!I61)</f>
-        <v>3.7957026157789647E-8</v>
+        <v>3.8287665892307243E-8</v>
       </c>
       <c r="I4" s="28">
         <f>SUM(Calculations!J49,Calculations!J55,Calculations!J61)</f>
-        <v>3.7717069860232141E-8</v>
+        <v>3.7805112321479254E-8</v>
       </c>
       <c r="J4" s="28">
         <f>SUM(Calculations!K49,Calculations!K55,Calculations!K61)</f>
-        <v>3.7396437294481469E-8</v>
+        <v>3.765441202979085E-8</v>
       </c>
       <c r="K4" s="28">
         <f>SUM(Calculations!L49,Calculations!L55,Calculations!L61)</f>
-        <v>3.7344871014411223E-8</v>
+        <v>3.7484027024007976E-8</v>
       </c>
       <c r="L4" s="28">
         <f>SUM(Calculations!M49,Calculations!M55,Calculations!M61)</f>
-        <v>3.7355095200280417E-8</v>
+        <v>3.7331298945699793E-8</v>
       </c>
       <c r="M4" s="28">
         <f>SUM(Calculations!N49,Calculations!N55,Calculations!N61)</f>
-        <v>3.7187854913945984E-8</v>
+        <v>3.7268157905839758E-8</v>
       </c>
       <c r="N4" s="28">
         <f>SUM(Calculations!O49,Calculations!O55,Calculations!O61)</f>
-        <v>3.6983471162150855E-8</v>
+        <v>3.7127503271735796E-8</v>
       </c>
       <c r="O4" s="28">
         <f>SUM(Calculations!P49,Calculations!P55,Calculations!P61)</f>
-        <v>3.6741121597956781E-8</v>
+        <v>3.6909881755452932E-8</v>
       </c>
       <c r="P4" s="28">
         <f>SUM(Calculations!Q49,Calculations!Q55,Calculations!Q61)</f>
-        <v>3.652764999956069E-8</v>
+        <v>3.6763363877106087E-8</v>
       </c>
       <c r="Q4" s="28">
         <f>SUM(Calculations!R49,Calculations!R55,Calculations!R61)</f>
-        <v>3.6503991970503002E-8</v>
+        <v>3.6608294905342332E-8</v>
       </c>
       <c r="R4" s="28">
         <f>SUM(Calculations!S49,Calculations!S55,Calculations!S61)</f>
-        <v>3.6454713135029713E-8</v>
+        <v>3.65686598579446E-8</v>
       </c>
       <c r="S4" s="28">
         <f>SUM(Calculations!T49,Calculations!T55,Calculations!T61)</f>
-        <v>3.646383710657876E-8</v>
+        <v>3.6587687405132364E-8</v>
       </c>
       <c r="T4" s="28">
         <f>SUM(Calculations!U49,Calculations!U55,Calculations!U61)</f>
-        <v>3.6555341736994743E-8</v>
+        <v>3.6676398178952397E-8</v>
       </c>
       <c r="U4" s="28">
         <f>SUM(Calculations!V49,Calculations!V55,Calculations!V61)</f>
-        <v>3.6611168793629211E-8</v>
+        <v>3.6720308296761374E-8</v>
       </c>
       <c r="V4" s="28">
         <f>SUM(Calculations!W49,Calculations!W55,Calculations!W61)</f>
-        <v>3.6524419640853654E-8</v>
+        <v>3.6689857879604365E-8</v>
       </c>
       <c r="W4" s="28">
         <f>SUM(Calculations!X49,Calculations!X55,Calculations!X61)</f>
-        <v>3.6274956128136681E-8</v>
+        <v>3.6370561962044375E-8</v>
       </c>
       <c r="X4" s="28">
         <f>SUM(Calculations!Y49,Calculations!Y55,Calculations!Y61)</f>
-        <v>3.6087139713799726E-8</v>
+        <v>3.618453934141425E-8</v>
       </c>
       <c r="Y4" s="28">
         <f>SUM(Calculations!Z49,Calculations!Z55,Calculations!Z61)</f>
-        <v>3.5975129274986296E-8</v>
+        <v>3.6078921812625026E-8</v>
       </c>
       <c r="Z4" s="28">
         <f>SUM(Calculations!AA49,Calculations!AA55,Calculations!AA61)</f>
-        <v>3.5925547700752817E-8</v>
+        <v>3.6017420896404737E-8</v>
       </c>
       <c r="AA4" s="28">
         <f>SUM(Calculations!AB49,Calculations!AB55,Calculations!AB61)</f>
-        <v>3.6015480378188342E-8</v>
+        <v>3.6086429632303422E-8</v>
       </c>
       <c r="AB4" s="28">
         <f>SUM(Calculations!AC49,Calculations!AC55,Calculations!AC61)</f>
-        <v>3.6145056020013418E-8</v>
+        <v>3.6241328558130178E-8</v>
       </c>
       <c r="AC4" s="28">
         <f>SUM(Calculations!AD49,Calculations!AD55,Calculations!AD61)</f>
-        <v>3.6250454340048288E-8</v>
+        <v>3.6414945648356179E-8</v>
       </c>
       <c r="AD4" s="28">
         <f>SUM(Calculations!AE49,Calculations!AE55,Calculations!AE61)</f>
-        <v>3.6322795084239807E-8</v>
+        <v>3.6525812767202976E-8</v>
       </c>
       <c r="AE4" s="28">
         <f>SUM(Calculations!AF49,Calculations!AF55,Calculations!AF61)</f>
-        <v>3.6397645357624208E-8</v>
+        <v>3.6560604599753893E-8</v>
       </c>
       <c r="AF4" s="28">
         <f>SUM(Calculations!AG49,Calculations!AG55,Calculations!AG61)</f>
-        <v>3.6593373518626685E-8</v>
+        <v>3.6700460475470092E-8</v>
       </c>
       <c r="AG4" s="28">
         <f>SUM(Calculations!AH49,Calculations!AH55,Calculations!AH61)</f>
-        <v>8.9706829293025634E-8</v>
+        <v>3.7184094734621651E-8</v>
       </c>
       <c r="AH4" s="28"/>
       <c r="AI4" s="28"/>

</xml_diff>

<commit_message>
Edit BS for 10 year PTC eligibility
</commit_message>
<xml_diff>
--- a/InputData/fuels/BS/BAU Subsidies.xlsx
+++ b/InputData/fuels/BS/BAU Subsidies.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1146" uniqueCount="646">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1150" uniqueCount="650">
   <si>
     <t>Source:</t>
   </si>
@@ -1988,6 +1988,18 @@
   </si>
   <si>
     <t>Section 9.2.2; Section 9.2.1, second paragraph</t>
+  </si>
+  <si>
+    <t>PTC Lifetime Adjustment</t>
+  </si>
+  <si>
+    <t>The PTC for wind is only available for 10 years of a project. We therefore multiply the PTC values by 10 and divide by the</t>
+  </si>
+  <si>
+    <t>average plant lifetime.</t>
+  </si>
+  <si>
+    <t>Average plant lifetime (see elec/BGCL)</t>
   </si>
 </sst>
 </file>
@@ -2754,10 +2766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E97"/>
+  <dimension ref="A1:E104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="A105" sqref="A105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3164,6 +3176,31 @@
     <row r="97" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A97" s="6" t="s">
         <v>367</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A99" s="29" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A100" s="6" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A101" s="6" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A103" s="6" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A104" s="6">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -3188,7 +3225,7 @@
   <dimension ref="A1:AI17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:AG14"/>
+      <selection activeCell="B8" sqref="B8:AG8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3954,100 +3991,132 @@
         <v>381</v>
       </c>
       <c r="B8" s="26">
-        <v>0</v>
+        <f>Calculations!C18*'Monetizing Tax Credit Penalty'!$A$30</f>
+        <v>1373199.8399999999</v>
       </c>
       <c r="C8" s="26">
-        <v>0</v>
+        <f>Calculations!D18*'Monetizing Tax Credit Penalty'!$A$30</f>
+        <v>1132390.5839999998</v>
       </c>
       <c r="D8" s="26">
-        <v>0</v>
+        <f>Calculations!E18*'Monetizing Tax Credit Penalty'!$A$30</f>
+        <v>1074674.6399999999</v>
       </c>
       <c r="E8" s="26">
-        <v>0</v>
+        <f>Calculations!F18*'Monetizing Tax Credit Penalty'!$A$30</f>
+        <v>1018003.8959999999</v>
       </c>
       <c r="F8" s="26">
-        <v>0</v>
+        <f>Calculations!G18*'Monetizing Tax Credit Penalty'!$A$30</f>
+        <v>829897.37599999993</v>
       </c>
       <c r="G8" s="26">
-        <v>0</v>
+        <f>Calculations!H18*'Monetizing Tax Credit Penalty'!$A$30</f>
+        <v>363327.6</v>
       </c>
       <c r="H8" s="26">
-        <v>0</v>
+        <f>Calculations!I18*'Monetizing Tax Credit Penalty'!$A$30</f>
+        <v>350641.14999999997</v>
       </c>
       <c r="I8" s="26">
-        <v>0</v>
+        <f>Calculations!J18*'Monetizing Tax Credit Penalty'!$A$30</f>
+        <v>338900.74</v>
       </c>
       <c r="J8" s="26">
-        <v>0</v>
+        <f>Calculations!K18*'Monetizing Tax Credit Penalty'!$A$30</f>
+        <v>328206.86999999994</v>
       </c>
       <c r="K8" s="26">
-        <v>0</v>
+        <f>Calculations!L18*'Monetizing Tax Credit Penalty'!$A$30</f>
+        <v>318516.65999999997</v>
       </c>
       <c r="L8" s="26">
-        <v>0</v>
+        <f>Calculations!M18*'Monetizing Tax Credit Penalty'!$A$30</f>
+        <v>309554.74</v>
       </c>
       <c r="M8" s="26">
-        <v>0</v>
+        <f>Calculations!N18*'Monetizing Tax Credit Penalty'!$A$30</f>
+        <v>301569.00999999995</v>
       </c>
       <c r="N8" s="26">
-        <v>0</v>
+        <f>Calculations!O18*'Monetizing Tax Credit Penalty'!$A$30</f>
+        <v>294371.19999999995</v>
       </c>
       <c r="O8" s="26">
-        <v>0</v>
+        <f>Calculations!P18*'Monetizing Tax Credit Penalty'!$A$30</f>
+        <v>287931.82999999996</v>
       </c>
       <c r="P8" s="26">
-        <v>0</v>
+        <f>Calculations!Q18*'Monetizing Tax Credit Penalty'!$A$30</f>
+        <v>282239.50999999995</v>
       </c>
       <c r="Q8" s="26">
-        <v>0</v>
+        <f>Calculations!R18*'Monetizing Tax Credit Penalty'!$A$30</f>
+        <v>277078.49999999994</v>
       </c>
       <c r="R8" s="26">
-        <v>0</v>
+        <f>Calculations!S18*'Monetizing Tax Credit Penalty'!$A$30</f>
+        <v>272656.5</v>
       </c>
       <c r="S8" s="26">
-        <v>0</v>
+        <f>Calculations!T18*'Monetizing Tax Credit Penalty'!$A$30</f>
+        <v>268685.40999999997</v>
       </c>
       <c r="T8" s="26">
-        <v>0</v>
+        <f>Calculations!U18*'Monetizing Tax Credit Penalty'!$A$30</f>
+        <v>265225.52999999997</v>
       </c>
       <c r="U8" s="26">
-        <v>0</v>
+        <f>Calculations!V18*'Monetizing Tax Credit Penalty'!$A$30</f>
+        <v>262286.24</v>
       </c>
       <c r="V8" s="26">
-        <v>0</v>
+        <f>Calculations!W18*'Monetizing Tax Credit Penalty'!$A$30</f>
+        <v>259722.14999999997</v>
       </c>
       <c r="W8" s="26">
-        <v>0</v>
+        <f>Calculations!X18*'Monetizing Tax Credit Penalty'!$A$30</f>
+        <v>257505.78999999998</v>
       </c>
       <c r="X8" s="26">
-        <v>0</v>
+        <f>Calculations!Y18*'Monetizing Tax Credit Penalty'!$A$30</f>
+        <v>255554.08</v>
       </c>
       <c r="Y8" s="26">
-        <v>0</v>
+        <f>Calculations!Z18*'Monetizing Tax Credit Penalty'!$A$30</f>
+        <v>253886.44999999998</v>
       </c>
       <c r="Z8" s="26">
-        <v>0</v>
+        <f>Calculations!AA18*'Monetizing Tax Credit Penalty'!$A$30</f>
+        <v>252480.78999999998</v>
       </c>
       <c r="AA8" s="26">
-        <v>0</v>
+        <f>Calculations!AB18*'Monetizing Tax Credit Penalty'!$A$30</f>
+        <v>251185.00999999998</v>
       </c>
       <c r="AB8" s="26">
-        <v>0</v>
+        <f>Calculations!AC18*'Monetizing Tax Credit Penalty'!$A$30</f>
+        <v>249954.21999999997</v>
       </c>
       <c r="AC8" s="26">
-        <v>0</v>
+        <f>Calculations!AD18*'Monetizing Tax Credit Penalty'!$A$30</f>
+        <v>248877.52999999997</v>
       </c>
       <c r="AD8" s="26">
-        <v>0</v>
+        <f>Calculations!AE18*'Monetizing Tax Credit Penalty'!$A$30</f>
+        <v>247712.39999999997</v>
       </c>
       <c r="AE8" s="26">
-        <v>0</v>
+        <f>Calculations!AF18*'Monetizing Tax Credit Penalty'!$A$30</f>
+        <v>246570.05</v>
       </c>
       <c r="AF8" s="26">
-        <v>0</v>
+        <f>Calculations!AG18*'Monetizing Tax Credit Penalty'!$A$30</f>
+        <v>245362.03999999998</v>
       </c>
       <c r="AG8" s="26">
-        <v>0</v>
+        <f>Calculations!AH18*'Monetizing Tax Credit Penalty'!$A$30</f>
+        <v>243934.93999999997</v>
       </c>
       <c r="AH8" s="26"/>
       <c r="AI8" s="26"/>
@@ -5983,8 +6052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X19"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -26364,7 +26433,7 @@
   <dimension ref="A1:AJ118"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A110" sqref="A110:XFD111"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -39279,28 +39348,28 @@
         <v>373</v>
       </c>
       <c r="B6" s="24">
-        <f>'Subsidies Paid'!I9*About!$A$84*1000*'Monetizing Tax Credit Penalty'!$A$30</f>
-        <v>13.839024708887294</v>
+        <f>'Subsidies Paid'!L9*About!$A$84*1000*'Monetizing Tax Credit Penalty'!$A$30*(10/About!$A$104)</f>
+        <v>2.0056557549112024</v>
       </c>
       <c r="C6" s="24">
-        <f>'Subsidies Paid'!J9*About!$A$84*1000*'Monetizing Tax Credit Penalty'!$A$30</f>
-        <v>11.071219767109838</v>
+        <f>'Subsidies Paid'!M9*About!$A$84*1000*'Monetizing Tax Credit Penalty'!$A$30*(10/About!$A$104)</f>
+        <v>3.0084836323668029</v>
       </c>
       <c r="D6" s="24">
-        <f>'Subsidies Paid'!K9*About!$A$84*1000*'Monetizing Tax Credit Penalty'!$A$30</f>
-        <v>8.3034148253323767</v>
+        <f>'Subsidies Paid'!N9*About!$A$84*1000*'Monetizing Tax Credit Penalty'!$A$30*(10/About!$A$104)</f>
+        <v>3.0084836323668029</v>
       </c>
       <c r="E6" s="24">
-        <f>'Subsidies Paid'!L9*About!$A$84*1000*'Monetizing Tax Credit Penalty'!$A$30</f>
-        <v>6.0169672647336077</v>
+        <f>D6</f>
+        <v>3.0084836323668029</v>
       </c>
       <c r="F6" s="24">
-        <f>'Subsidies Paid'!M9*About!$A$84*1000*'Monetizing Tax Credit Penalty'!$A$30</f>
-        <v>9.0254508971004093</v>
+        <f t="shared" ref="F6:G6" si="0">E6</f>
+        <v>3.0084836323668029</v>
       </c>
       <c r="G6" s="24">
-        <f>'Subsidies Paid'!N9*About!$A$84*1000*'Monetizing Tax Credit Penalty'!$A$30</f>
-        <v>9.0254508971004093</v>
+        <f t="shared" si="0"/>
+        <v>3.0084836323668029</v>
       </c>
       <c r="H6" s="24">
         <f>'Subsidies Paid'!O9*About!$A$84*1000*'Monetizing Tax Credit Penalty'!$A$30</f>
@@ -40029,131 +40098,131 @@
         <v>369</v>
       </c>
       <c r="B13" s="24">
-        <f t="shared" ref="B13:AG13" si="0">B2</f>
+        <f t="shared" ref="B13:AG13" si="1">B2</f>
         <v>0.31269731656692296</v>
       </c>
       <c r="C13" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.34285778860529786</v>
       </c>
       <c r="D13" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.3622498402976298</v>
       </c>
       <c r="E13" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.37598025289549725</v>
       </c>
       <c r="F13" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.40646738989562903</v>
       </c>
       <c r="G13" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.41415229287630889</v>
       </c>
       <c r="H13" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.42323668613563886</v>
       </c>
       <c r="I13" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.39946945449758892</v>
       </c>
       <c r="J13" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.40009106872906414</v>
       </c>
       <c r="K13" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.40096047140548391</v>
       </c>
       <c r="L13" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.40118376652093307</v>
       </c>
       <c r="M13" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.40197253766231777</v>
       </c>
       <c r="N13" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.40455090151073586</v>
       </c>
       <c r="O13" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.40526200782514737</v>
       </c>
       <c r="P13" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.40191554233607107</v>
       </c>
       <c r="Q13" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.40537862357361099</v>
       </c>
       <c r="R13" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.41050739265180025</v>
       </c>
       <c r="S13" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.41390216809681823</v>
       </c>
       <c r="T13" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.41454867472941087</v>
       </c>
       <c r="U13" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.4196434670496747</v>
       </c>
       <c r="V13" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.42276478981633353</v>
       </c>
       <c r="W13" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.424336572612173</v>
       </c>
       <c r="X13" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.42632767697024587</v>
       </c>
       <c r="Y13" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.42810908238255907</v>
       </c>
       <c r="Z13" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.42964122355639361</v>
       </c>
       <c r="AA13" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.42964272552180816</v>
       </c>
       <c r="AB13" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.43184498257581788</v>
       </c>
       <c r="AC13" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.4277449404086352</v>
       </c>
       <c r="AD13" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.42808186375576363</v>
       </c>
       <c r="AE13" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.42853720191730743</v>
       </c>
       <c r="AF13" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.4303143276189097</v>
       </c>
       <c r="AG13" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.42845475850445314</v>
       </c>
       <c r="AH13" s="24"/>
@@ -40164,12 +40233,12 @@
         <v>370</v>
       </c>
       <c r="B14" s="24">
-        <f>'Subsidies Paid'!I10*About!$A$84*1000*'Monetizing Tax Credit Penalty'!$A$30</f>
-        <v>13.839024708887294</v>
+        <f>'Subsidies Paid'!L10*About!$A$84*1000*'Monetizing Tax Credit Penalty'!$A$30*(10/About!$A$104)</f>
+        <v>2.0056557549112024</v>
       </c>
       <c r="C14" s="24">
-        <f>'Subsidies Paid'!J10*About!$A$84*1000*'Monetizing Tax Credit Penalty'!$A$30</f>
-        <v>11.071219767109838</v>
+        <f>'Subsidies Paid'!M10*About!$A$84*1000*'Monetizing Tax Credit Penalty'!$A$30*(10/About!$A$104)</f>
+        <v>3.0084836323668029</v>
       </c>
       <c r="D14" s="24">
         <f>'Subsidies Paid'!N10*About!$A$84*1000*'Monetizing Tax Credit Penalty'!$A$30</f>
@@ -40287,123 +40356,123 @@
         <v>0</v>
       </c>
       <c r="D15" s="8">
-        <f t="shared" ref="D15:AG15" si="1">D11</f>
+        <f t="shared" ref="D15:AG15" si="2">D11</f>
         <v>0</v>
       </c>
       <c r="E15" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F15" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G15" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H15" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I15" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J15" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K15" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L15" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M15" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N15" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O15" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P15" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q15" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R15" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="S15" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="T15" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U15" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="V15" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="W15" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="X15" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Y15" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z15" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AA15" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB15" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AC15" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AD15" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AE15" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AF15" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AG15" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH15" s="8"/>
@@ -40422,123 +40491,123 @@
         <v>0</v>
       </c>
       <c r="D16" s="8">
-        <f t="shared" ref="D16:AG16" si="2">D11</f>
+        <f t="shared" ref="D16:AG16" si="3">D11</f>
         <v>0</v>
       </c>
       <c r="E16" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F16" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G16" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H16" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I16" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J16" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K16" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L16" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M16" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N16" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O16" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P16" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q16" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R16" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S16" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T16" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U16" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="V16" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W16" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="X16" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Y16" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Z16" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AA16" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AB16" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC16" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AD16" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AE16" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF16" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AG16" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AH16" s="8"/>

</xml_diff>